<commit_message>
all set login and logout
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>medname</t>
   </si>
@@ -40,19 +40,28 @@
     <t>jalebi</t>
   </si>
   <si>
+    <t>siddhu</t>
+  </si>
+  <si>
+    <t>siddharth</t>
+  </si>
+  <si>
     <t>2024-03-12</t>
   </si>
   <si>
     <t>2024-03-13</t>
   </si>
   <si>
+    <t>2024-03-01</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>2024-03-14</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -410,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +447,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -447,7 +456,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -455,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -464,7 +473,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -472,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -481,7 +490,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -489,7 +498,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -498,7 +507,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -506,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -515,7 +524,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -523,16 +532,50 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>